<commit_message>
add results by subject area
</commit_message>
<xml_diff>
--- a/results/results-chaos.xlsx
+++ b/results/results-chaos.xlsx
@@ -795,7 +795,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MAPE</t>
+          <t>MAE</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -808,7 +808,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MAE</t>
+          <t>MAPE</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -847,7 +847,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>precision</t>
+          <t>nRMSE</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -860,7 +860,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>RMSPE</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -873,7 +873,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>RMdSPE</t>
+          <t>accuracy</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -886,7 +886,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>RMSPE</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -899,7 +899,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>nRMSE</t>
+          <t>RMSLE</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -912,7 +912,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RMSLE</t>
+          <t>precision</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -925,7 +925,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>accuracy</t>
+          <t>RMdSPE</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1252,7 +1252,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>note factors that were not accounted for in their model</t>
+          <t>data</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1265,7 +1265,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>data</t>
+          <t>note factors that were not accounted for in their model</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1497,7 +1497,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>policy</t>
+          <t>climate</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1510,7 +1510,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>climate</t>
+          <t>policy</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1523,7 +1523,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>mobility</t>
+          <t>demographics</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1536,7 +1536,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>demographics</t>
+          <t>mobility</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1585,7 +1585,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>General Physics and Astronomy</t>
+          <t>Statistical and Nonlinear Physics</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1598,7 +1598,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>General Mathematics</t>
+          <t>General Physics and Astronomy</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1611,7 +1611,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Statistical and Nonlinear Physics</t>
+          <t>General Mathematics</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1973,7 +1973,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>state</t>
+          <t>county or smaller</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1986,7 +1986,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>county or smaller</t>
+          <t>state</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2162,7 +2162,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>symptomatic cases</t>
+          <t>end dates of pandemic</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2188,7 +2188,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ventilators</t>
+          <t>peak cases date</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2201,7 +2201,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>peak deaths</t>
+          <t>ventilators</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2214,7 +2214,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>peak cases date</t>
+          <t>symptomatic cases</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2227,7 +2227,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>attack rate</t>
+          <t>peak deaths</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2240,7 +2240,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>end dates of pandemic</t>
+          <t>total deaths</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -2253,7 +2253,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>total deaths</t>
+          <t>attack rate</t>
         </is>
       </c>
       <c r="B13" t="n">

</xml_diff>